<commit_message>
Update processed and raw data files, add outputs
Added new raw energy and input files, updated processed CSV and analysis results, and included new output diagnostics and figures. These changes support expanded data coverage and improved analysis for the sisepuede project.
</commit_message>
<xml_diff>
--- a/data/processed/sisepuede_analysis_results.xlsx
+++ b/data/processed/sisepuede_analysis_results.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Baseline_Emissions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,6 +426,1285 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:DJ3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>time_period</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_biofuels</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_biogas</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_biomass</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_coal</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_coal_deposits</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_coke</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_crude</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_diesel</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_electricity</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_furnace_gas</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_gasoline</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_geothermal</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_hydrocarbon_gas_liquids</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_hydrogen</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_water</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_kerosene</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_natural_gas_liquid</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_natural_gas_unprocessed</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_nuclear</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_ocean</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_oil</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_other</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_solar</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_waste</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ef_enfu_combustion_tonne_co2_per_tj_fuel_wind</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_distribution_tonne_co2_per_m3_fuel_natural_gas</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_shrublands_to_other_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>ef_frst_sequestration_secondary_kt_co2_ha</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_production_flaring_tonne_co2_per_m3_fuel_natural_gas</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_production_flaring_tonne_co2_per_m3_fuel_oil</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_production_fugitive_tonne_co2_per_m3_fuel_coal</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_production_fugitive_tonne_co2_per_m3_fuel_natural_gas</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_production_fugitive_tonne_co2_per_m3_fuel_oil</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>ef_frst_sequestration_young_secondary_kt_co2_ha</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_production_venting_tonne_co2_per_m3_fuel_oil</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_transmission_tonne_co2_per_m3_fuel_natural_gas</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>ef_fgtv_transmission_tonne_co2_per_m3_fuel_oil</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_other_to_flooded_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_other_to_wetlands_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>ef_ippu_tonne_co2_per_tonne_product_use_product_use_lubricants</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>ef_ippu_tonne_co2_per_tonne_product_use_product_use_paraffin_wax</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>ef_ippu_tonne_co2_per_tonne_production_cement_clinker</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>ef_ippu_tonne_co2_per_tonne_production_chemicals</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>ef_ippu_tonne_co2_per_tonne_production_lime_and_carbonite</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_other_to_forests_secondary_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_croplands_to_other_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>energy_intensity_ccsq_direct_air_capture_gj_per_tonne_co2</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_wetlands_to_forests_mangroves_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>frac_ippu_production_with_co2_capture_chemicals</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>frac_ippu_production_with_co2_capture_lime_and_carbonite</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>frac_ippu_production_with_co2_capture_plastic</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>ef_lndu_conv_wetlands_to_other_gg_co2_ha</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>gasrf_ippu_co2_capture_cement</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>gasrf_ippu_co2_capture_chemicals</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>gasrf_ippu_co2_capture_glass</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>gasrf_ippu_co2_capture_lime_and_carbonite</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>gasrf_ippu_co2_capture_metals</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>gasrf_ippu_co2_capture_plastic</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>limit_gnrl_annual_emissions_mt_ch4</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>limit_gnrl_annual_emissions_mt_co2</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>limit_gnrl_annual_emissions_mt_n2o</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_hydrogen_gasification_tonne_co2_per_tj</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_hydrogen_reformation_ccs_tonne_co2_per_tj</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_natural_gas_liquefaction_tonne_ch4_per_tj</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_natural_gas_liquefaction_tonne_co2_per_tj</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_natural_gas_liquefaction_tonne_n2o_per_tj</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_petroleum_refinement_tonne_ch4_per_tj</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_petroleum_refinement_tonne_co2_per_tj</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_fuel_production_fp_petroleum_refinement_tonne_n2o_per_tj</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_biogas_ch4</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_biogas_co2</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_biogas_n2o</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_biomass_ch4</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_biomass_co2</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_biomass_n2o</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_coal_ccs_ch4</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_coal_ccs_co2</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_coal_ccs_n2o</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_coal_ch4</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_coal_co2</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_coal_n2o</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_gas_ccs_ch4</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_fp_hydrogen_reformation_ccs_co2</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_gas_ccs_n2o</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_gas_ch4</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_gas_co2</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_gas_n2o</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_geothermal_ch4</t>
+        </is>
+      </c>
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_geothermal_co2</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_geothermal_n2o</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_hydropower_ch4</t>
+        </is>
+      </c>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_hydropower_co2</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_hydropower_n2o</t>
+        </is>
+      </c>
+      <c r="CQ1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_nuclear_ch4</t>
+        </is>
+      </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_nuclear_co2</t>
+        </is>
+      </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_nuclear_n2o</t>
+        </is>
+      </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_ocean_ch4</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_ocean_co2</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_ocean_n2o</t>
+        </is>
+      </c>
+      <c r="CW1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_oil_ch4</t>
+        </is>
+      </c>
+      <c r="CX1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_oil_co2</t>
+        </is>
+      </c>
+      <c r="CY1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_oil_n2o</t>
+        </is>
+      </c>
+      <c r="CZ1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_solar_ch4</t>
+        </is>
+      </c>
+      <c r="DA1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_solar_co2</t>
+        </is>
+      </c>
+      <c r="DB1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_solar_n2o</t>
+        </is>
+      </c>
+      <c r="DC1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_waste_incineration_ch4</t>
+        </is>
+      </c>
+      <c r="DD1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_waste_incineration_co2</t>
+        </is>
+      </c>
+      <c r="DE1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_waste_incineration_n2o</t>
+        </is>
+      </c>
+      <c r="DF1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_wind_ch4</t>
+        </is>
+      </c>
+      <c r="DG1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_wind_co2</t>
+        </is>
+      </c>
+      <c r="DH1" s="1" t="inlineStr">
+        <is>
+          <t>nemomod_entc_emissions_activity_ratio_scalar_pp_wind_n2o</t>
+        </is>
+      </c>
+      <c r="DI1" s="1" t="inlineStr">
+        <is>
+          <t>qty_ccsq_mt_co2_captured_sequestered_by_direct_air_capture</t>
+        </is>
+      </c>
+      <c r="DJ1" s="1" t="inlineStr">
+        <is>
+          <t>total_emissions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B3" t="n">
+        <v>73.73333333333331</v>
+      </c>
+      <c r="C3" t="n">
+        <v>54.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>112</v>
+      </c>
+      <c r="E3" t="n">
+        <v>94.59999999999999</v>
+      </c>
+      <c r="F3" t="n">
+        <v>97.01666666666659</v>
+      </c>
+      <c r="G3" t="n">
+        <v>103.833333333333</v>
+      </c>
+      <c r="H3" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>221</v>
+      </c>
+      <c r="L3" t="n">
+        <v>69.76666666666659</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="R3" t="n">
+        <v>60.15</v>
+      </c>
+      <c r="S3" t="n">
+        <v>60.15</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>75.34999999999999</v>
+      </c>
+      <c r="W3" t="n">
+        <v>95.06666666666661</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>100.37</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>8.449852069711041e-08</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.000141052701680675</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.0514151820857197</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>4.89277622940513e-06</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.0399749921826133</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>6.17126699340616e-05</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.0102490704319759</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.00516330912334678</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.00212132034355964</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>6.25286521830155e-09</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1.395e-06</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.000173571428571428</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.00396543</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.848907407407407</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.03741</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>12.858</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>18.535</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>2.236</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>167.025</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>74.266037735849</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>3.358e-05</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>1.0099</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>5.877e-06</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0.000260869565217391</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>6.37391304347825</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>5.21739130434782e-05</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CY3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CZ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ3" t="n">
+        <v>846.2464593733737</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -462,7 +1742,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +1752,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +1762,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +1772,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>